<commit_message>
update data transformation selection
</commit_message>
<xml_diff>
--- a/result_files/final_result_dataAug_T_lapras_ST1_NT1.xlsx
+++ b/result_files/final_result_dataAug_T_lapras_ST1_NT1.xlsx
@@ -450,10 +450,10 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>0.7987179487179488</v>
+        <v>0.8510355029585798</v>
       </c>
       <c r="C2" t="n">
-        <v>0.1202247692976583</v>
+        <v>0.1012245750502546</v>
       </c>
     </row>
     <row r="3">
@@ -461,10 +461,10 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>0.8934911242603552</v>
+        <v>0.7795857988165681</v>
       </c>
       <c r="C3" t="n">
-        <v>0.0315581854043392</v>
+        <v>0.09496585691618256</v>
       </c>
     </row>
     <row r="4">
@@ -472,10 +472,10 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>0.9948717948717949</v>
+        <v>0.8126725838264299</v>
       </c>
       <c r="C4" t="n">
-        <v>0.005415988251576313</v>
+        <v>0.1780890680725701</v>
       </c>
     </row>
     <row r="5">
@@ -483,10 +483,10 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>0.5175542406311637</v>
+        <v>0.6672090729783038</v>
       </c>
       <c r="C5" t="n">
-        <v>0.07776032500564814</v>
+        <v>0.1677474570688943</v>
       </c>
     </row>
     <row r="6">
@@ -494,10 +494,10 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>0.8994082840236686</v>
+        <v>0.8407914201183431</v>
       </c>
       <c r="C6" t="n">
-        <v>0.0769332108140434</v>
+        <v>0.06079329372474069</v>
       </c>
     </row>
   </sheetData>

</xml_diff>